<commit_message>
Facturas y documentacion recibida
</commit_message>
<xml_diff>
--- a/FASE III - Informe/9100 Evaluacion de evidencia/9110 Revision analitica final/9111 Revision analitica final.xlsx
+++ b/FASE III - Informe/9100 Evaluacion de evidencia/9110 Revision analitica final/9111 Revision analitica final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Almeida\Documents\GitHub\TELCODATA\FASE III - Informe\9100 Evaluacion de evidencia\9110 Revision analitica final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5749E1C9-1FC7-4986-B2CD-E421BA6E3ECC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B7708B-BC99-4B82-AAF9-A9F933409033}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BG" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="469">
   <si>
     <t xml:space="preserve"> ACTIVOS</t>
   </si>
@@ -1629,7 +1629,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1698,6 +1698,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2041,12 +2045,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A5" sqref="A5"/>
       <selection pane="topRight" activeCell="C5" sqref="C5"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
+      <selection pane="bottomRight" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2215,7 +2219,7 @@
       </c>
       <c r="C12" s="17">
         <f>+'BC 20'!F20</f>
-        <v>114096.31</v>
+        <v>142550.39000000001</v>
       </c>
       <c r="D12" s="17">
         <v>137808</v>
@@ -2225,11 +2229,11 @@
       </c>
       <c r="F12" s="17">
         <f t="shared" si="0"/>
-        <v>-23711.690000000002</v>
+        <v>4742.390000000014</v>
       </c>
       <c r="G12" s="26">
         <f t="shared" si="1"/>
-        <v>-0.17206323290375017</v>
+        <v>3.4413023917334362E-2</v>
       </c>
       <c r="H12" s="16"/>
     </row>
@@ -2239,7 +2243,7 @@
       </c>
       <c r="C13" s="17">
         <f>+'BC 20'!H32</f>
-        <v>221771.13</v>
+        <v>93444.75</v>
       </c>
       <c r="D13" s="17">
         <f>+'BC19'!H34</f>
@@ -2250,11 +2254,11 @@
       </c>
       <c r="F13" s="17">
         <f t="shared" si="0"/>
-        <v>140057.12</v>
+        <v>11730.740000000005</v>
       </c>
       <c r="G13" s="26">
         <f t="shared" si="1"/>
-        <v>1.7139915174888616</v>
+        <v>0.14355849137742727</v>
       </c>
       <c r="H13" s="16"/>
     </row>
@@ -2264,7 +2268,7 @@
       </c>
       <c r="C14" s="14">
         <f>SUM(C7:C13)</f>
-        <v>582857.22</v>
+        <v>482984.92</v>
       </c>
       <c r="D14" s="14">
         <f>SUM(D7:D13)</f>
@@ -2276,11 +2280,11 @@
       </c>
       <c r="F14" s="14">
         <f t="shared" si="0"/>
-        <v>24834.349999999977</v>
+        <v>-75037.950000000012</v>
       </c>
       <c r="G14" s="28">
         <f t="shared" si="1"/>
-        <v>4.4504179550920515E-2</v>
+        <v>-0.13447110151596478</v>
       </c>
       <c r="H14" s="16"/>
     </row>
@@ -2290,7 +2294,7 @@
       </c>
       <c r="C15" s="14">
         <f>+C14</f>
-        <v>582857.22</v>
+        <v>482984.92</v>
       </c>
       <c r="D15" s="14">
         <f>+D14</f>
@@ -2302,11 +2306,11 @@
       </c>
       <c r="F15" s="14">
         <f t="shared" si="0"/>
-        <v>24834.349999999977</v>
+        <v>-75037.950000000012</v>
       </c>
       <c r="G15" s="28">
         <f t="shared" si="1"/>
-        <v>4.4504179550920515E-2</v>
+        <v>-0.13447110151596478</v>
       </c>
       <c r="H15" s="16"/>
     </row>
@@ -2345,10 +2349,7 @@
       <c r="B19" s="16" t="s">
         <v>464</v>
       </c>
-      <c r="C19" s="17">
-        <f>-'BC19'!F65</f>
-        <v>0</v>
-      </c>
+      <c r="C19" s="17"/>
       <c r="D19" s="17"/>
       <c r="E19" s="17">
         <v>57028</v>
@@ -2362,7 +2363,7 @@
         <v>465</v>
       </c>
       <c r="C20" s="17">
-        <f>-'BC 20'!F57</f>
+        <f>-'BC 20'!F58</f>
         <v>0</v>
       </c>
       <c r="D20" s="17">
@@ -2372,7 +2373,7 @@
         <v>168381</v>
       </c>
       <c r="F20" s="17">
-        <f t="shared" ref="F19:F24" si="2">+C20-D20</f>
+        <f t="shared" ref="F20:F24" si="2">+C20-D20</f>
         <v>-23852</v>
       </c>
       <c r="G20" s="26">
@@ -2386,7 +2387,6 @@
         <v>461</v>
       </c>
       <c r="C21" s="17">
-        <f>-'BC19'!F68</f>
         <v>0</v>
       </c>
       <c r="D21" s="17">
@@ -2421,7 +2421,7 @@
         <v>463</v>
       </c>
       <c r="C23" s="17">
-        <f>-'BC 20'!G43</f>
+        <f>-'BC 20'!G44</f>
         <v>1213.1300000000001</v>
       </c>
       <c r="D23" s="17">
@@ -2491,7 +2491,7 @@
         <v>241</v>
       </c>
       <c r="C27" s="17">
-        <f>-'BC 20'!F71</f>
+        <f>-'BC 20'!F72</f>
         <v>20000</v>
       </c>
       <c r="D27" s="17">
@@ -2516,7 +2516,7 @@
         <v>242</v>
       </c>
       <c r="C28" s="17">
-        <f>-'BC 20'!E77</f>
+        <f>-'BC 20'!E78</f>
         <v>142203.51</v>
       </c>
       <c r="D28" s="17">
@@ -2541,7 +2541,7 @@
         <v>243</v>
       </c>
       <c r="C29" s="17">
-        <f>-'BC 20'!E78</f>
+        <f>-'BC 20'!E79</f>
         <v>204380.95</v>
       </c>
       <c r="D29" s="17">
@@ -2566,8 +2566,8 @@
         <v>244</v>
       </c>
       <c r="C30" s="17">
-        <f>-'BC 20'!J85</f>
-        <v>153332.70000000001</v>
+        <f>-'BC 20'!J86</f>
+        <v>53460.399999999994</v>
       </c>
       <c r="D30" s="17">
         <v>126579</v>
@@ -2577,11 +2577,11 @@
       </c>
       <c r="F30" s="17">
         <f t="shared" si="4"/>
-        <v>26753.700000000012</v>
+        <v>-73118.600000000006</v>
       </c>
       <c r="G30" s="26">
         <f t="shared" si="5"/>
-        <v>0.21135970421633929</v>
+        <v>-0.5776519011842407</v>
       </c>
       <c r="H30" s="16"/>
     </row>
@@ -2590,7 +2590,7 @@
         <v>245</v>
       </c>
       <c r="C31" s="17">
-        <f>-'BC 20'!I79</f>
+        <f>-'BC 20'!I80</f>
         <v>61726.93</v>
       </c>
       <c r="D31" s="17">
@@ -2617,7 +2617,7 @@
       </c>
       <c r="C32" s="14">
         <f>SUM(C27:C31)</f>
-        <v>581644.09000000008</v>
+        <v>481771.79</v>
       </c>
       <c r="D32" s="14">
         <f>SUM(D27:D31)</f>
@@ -2629,11 +2629,11 @@
       </c>
       <c r="F32" s="14">
         <f t="shared" si="4"/>
-        <v>153333.05000000005</v>
+        <v>53460.749999999942</v>
       </c>
       <c r="G32" s="28">
         <f t="shared" si="5"/>
-        <v>0.35799462465408322</v>
+        <v>0.12481758583668527</v>
       </c>
       <c r="H32" s="16"/>
     </row>
@@ -2643,7 +2643,7 @@
       </c>
       <c r="C33" s="18">
         <f>+C24+C32</f>
-        <v>582857.22000000009</v>
+        <v>482984.92</v>
       </c>
       <c r="D33" s="18">
         <f>+D24+D32</f>
@@ -2655,17 +2655,23 @@
       </c>
       <c r="F33" s="14">
         <f t="shared" si="4"/>
-        <v>24834.180000000051</v>
+        <v>-75038.120000000054</v>
       </c>
       <c r="G33" s="27">
         <f t="shared" si="5"/>
-        <v>4.4503861345940213E-2</v>
+        <v>-0.13447136519667727</v>
       </c>
       <c r="H33" s="19"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
+      <c r="C34" s="10">
+        <f>+C33-C15</f>
+        <v>0</v>
+      </c>
+      <c r="D34" s="10">
+        <f>+D33-D15</f>
+        <v>0.17000000004190952</v>
+      </c>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
@@ -2676,7 +2682,7 @@
       </c>
       <c r="C35" s="30">
         <f>+C14/C24</f>
-        <v>480.45734587389637</v>
+        <v>398.13121429690136</v>
       </c>
       <c r="D35" s="30">
         <f>+D14/D24</f>
@@ -2698,7 +2704,7 @@
       </c>
       <c r="C36" s="31">
         <f>+C24/C32</f>
-        <v>2.0856912686931968E-3</v>
+        <v>2.518059432246957E-3</v>
       </c>
       <c r="D36" s="31">
         <f>+D24/D32</f>
@@ -2777,10 +2783,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2838,7 +2844,7 @@
         <v>422</v>
       </c>
       <c r="C6" s="17">
-        <f>-'BC 20'!J90</f>
+        <f>-'BC 20'!J91</f>
         <v>547020</v>
       </c>
       <c r="D6" s="17">
@@ -2862,8 +2868,8 @@
         <v>250</v>
       </c>
       <c r="C7" s="17">
-        <f>'BC 20'!E101</f>
-        <v>264271.33</v>
+        <f>'BC 20'!E102</f>
+        <v>392066.26</v>
       </c>
       <c r="D7" s="17">
         <v>254206</v>
@@ -2872,12 +2878,12 @@
         <v>596245</v>
       </c>
       <c r="F7" s="17">
-        <f t="shared" ref="F7:F9" si="0">+C7-D7</f>
-        <v>10065.330000000016</v>
+        <f t="shared" ref="F7:F8" si="0">+C7-D7</f>
+        <v>137860.26</v>
       </c>
       <c r="G7" s="45">
         <f t="shared" ref="G7:G8" si="1">+F7/D7</f>
-        <v>3.959517084569214E-2</v>
+        <v>0.54231709715742349</v>
       </c>
       <c r="H7" s="16"/>
     </row>
@@ -2887,7 +2893,7 @@
       </c>
       <c r="C8" s="20">
         <f>+C6-C7</f>
-        <v>282748.67</v>
+        <v>154953.74</v>
       </c>
       <c r="D8" s="20">
         <f>+D6-D7</f>
@@ -2899,11 +2905,11 @@
       </c>
       <c r="F8" s="20">
         <f t="shared" si="0"/>
-        <v>-28405.330000000016</v>
+        <v>-156200.26</v>
       </c>
       <c r="G8" s="45">
         <f t="shared" si="1"/>
-        <v>-9.1290261413962265E-2</v>
+        <v>-0.50200305957821534</v>
       </c>
       <c r="H8" s="16"/>
     </row>
@@ -2911,7 +2917,7 @@
       <c r="B9" s="16"/>
       <c r="C9" s="24">
         <f>+C8/C6</f>
-        <v>0.51688908997842853</v>
+        <v>0.28326887499542974</v>
       </c>
       <c r="D9" s="24">
         <f>+D8/D6</f>
@@ -2931,7 +2937,7 @@
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
       <c r="F10" s="17">
-        <f t="shared" ref="F8:F19" si="2">+D10-E10</f>
+        <f t="shared" ref="F10:F19" si="2">+D10-E10</f>
         <v>0</v>
       </c>
       <c r="G10" s="45"/>
@@ -2942,8 +2948,8 @@
         <v>252</v>
       </c>
       <c r="C11" s="17">
-        <f>'BC 20'!F106-'BC 20'!E107</f>
-        <v>128331.45</v>
+        <f>'BC 20'!F107-'BC 20'!E116-'BC 20'!E115</f>
+        <v>84885.209999999992</v>
       </c>
       <c r="D11" s="17">
         <v>148706</v>
@@ -2954,11 +2960,11 @@
       </c>
       <c r="F11" s="17">
         <f>+C11-D11</f>
-        <v>-20374.550000000003</v>
+        <v>-63820.790000000008</v>
       </c>
       <c r="G11" s="45">
         <f>+F11/D11</f>
-        <v>-0.13701229271179377</v>
+        <v>-0.42917427676085707</v>
       </c>
       <c r="H11" s="16"/>
     </row>
@@ -2966,7 +2972,7 @@
       <c r="B12" s="16"/>
       <c r="C12" s="24">
         <f>+C11/C6</f>
-        <v>0.23460102007239222</v>
+        <v>0.1551775255018098</v>
       </c>
       <c r="D12" s="24">
         <f>+D11/D6</f>
@@ -2986,7 +2992,7 @@
       </c>
       <c r="C13" s="47">
         <f>+C8-C11</f>
-        <v>154417.21999999997</v>
+        <v>70068.53</v>
       </c>
       <c r="D13" s="47">
         <f>+D8-D11</f>
@@ -2995,11 +3001,11 @@
       <c r="E13" s="43"/>
       <c r="F13" s="20">
         <f>+C13-D13</f>
-        <v>-8030.7800000000279</v>
+        <v>-92379.47</v>
       </c>
       <c r="G13" s="45">
         <f>+F13/D13</f>
-        <v>-4.9436004136708532E-2</v>
+        <v>-0.5686710208805279</v>
       </c>
       <c r="H13" s="16"/>
     </row>
@@ -3017,8 +3023,8 @@
         <v>253</v>
       </c>
       <c r="C15" s="17">
-        <f>-'BC 20'!E107-'BC 20'!E119</f>
-        <v>-74.16</v>
+        <f>-'BC 20'!E115-'BC 20'!E120</f>
+        <v>-207.74</v>
       </c>
       <c r="D15" s="17">
         <v>-120</v>
@@ -3028,11 +3034,11 @@
       </c>
       <c r="F15" s="17">
         <f>+C15-D15</f>
-        <v>45.84</v>
+        <v>-87.740000000000009</v>
       </c>
       <c r="G15" s="45">
         <f>+F15/D15</f>
-        <v>-0.38200000000000001</v>
+        <v>0.73116666666666674</v>
       </c>
       <c r="H15" s="23"/>
     </row>
@@ -3041,7 +3047,7 @@
         <v>467</v>
       </c>
       <c r="C16" s="17">
-        <f>-'BC 20'!E125-'BC 20'!E130</f>
+        <f>-'BC 20'!E126-'BC 20'!E131</f>
         <v>-1010.36</v>
       </c>
       <c r="D16" s="17"/>
@@ -3056,7 +3062,7 @@
       </c>
       <c r="C17" s="20">
         <f>SUM(C13:C16)</f>
-        <v>153332.69999999998</v>
+        <v>68850.429999999993</v>
       </c>
       <c r="D17" s="20">
         <f>SUM(D13:D16)</f>
@@ -3068,11 +3074,11 @@
       </c>
       <c r="F17" s="20">
         <f>+C17-D17</f>
-        <v>-8995.3000000000175</v>
+        <v>-93477.57</v>
       </c>
       <c r="G17" s="45">
         <f>+F17/D17</f>
-        <v>-5.5414346261889617E-2</v>
+        <v>-0.57585610615543836</v>
       </c>
       <c r="H17" s="16"/>
     </row>
@@ -3080,7 +3086,7 @@
       <c r="B18" s="16"/>
       <c r="C18" s="24">
         <f>+C17/C6</f>
-        <v>0.28030547329165295</v>
+        <v>0.12586455705458666</v>
       </c>
       <c r="D18" s="24">
         <f>+D17/D6</f>
@@ -3118,7 +3124,10 @@
       <c r="B20" s="16" t="s">
         <v>256</v>
       </c>
-      <c r="C20" s="17"/>
+      <c r="C20" s="17">
+        <f>+'BC 20'!E116</f>
+        <v>15390.03</v>
+      </c>
       <c r="D20" s="17">
         <v>35749</v>
       </c>
@@ -3127,11 +3136,11 @@
       </c>
       <c r="F20" s="17">
         <f t="shared" ref="F20:F21" si="3">+C20-D20</f>
-        <v>-35749</v>
+        <v>-20358.97</v>
       </c>
       <c r="G20" s="45">
         <f t="shared" ref="G20:G21" si="4">+F20/D20</f>
-        <v>-1</v>
+        <v>-0.56949760832470842</v>
       </c>
       <c r="H20" s="16"/>
     </row>
@@ -3141,7 +3150,7 @@
       </c>
       <c r="C21" s="14">
         <f>+C17-C20</f>
-        <v>153332.69999999998</v>
+        <v>53460.399999999994</v>
       </c>
       <c r="D21" s="14">
         <f>+D17-D20</f>
@@ -3152,18 +3161,18 @@
       </c>
       <c r="F21" s="14">
         <f t="shared" si="3"/>
-        <v>26753.699999999983</v>
+        <v>-73118.600000000006</v>
       </c>
       <c r="G21" s="45">
         <f t="shared" si="4"/>
-        <v>0.21135970421633907</v>
+        <v>-0.5776519011842407</v>
       </c>
       <c r="H21" s="19"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C22" s="25">
         <f>+C21/C6</f>
-        <v>0.28030547329165295</v>
+        <v>9.7730247522942473E-2</v>
       </c>
       <c r="D22" s="25">
         <f>+D21/D6</f>
@@ -3174,6 +3183,9 @@
         <v>7.8542339219802332E-2</v>
       </c>
       <c r="G22" s="46"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3183,19 +3195,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9396899F-A8AB-4DBF-AFA4-160DCFF68FAC}">
-  <dimension ref="A2:J132"/>
+  <dimension ref="A2:J133"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="B132" sqref="B132"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
     <col min="4" max="4" width="2.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="11.5703125" style="48" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.35">
@@ -3229,8 +3241,13 @@
       <c r="D7" s="3">
         <v>1</v>
       </c>
-      <c r="J7" s="5">
-        <v>582857.22</v>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49">
+        <v>482984.92</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3246,9 +3263,14 @@
       <c r="D8" s="3">
         <v>2</v>
       </c>
-      <c r="I8" s="5">
-        <v>361086.09</v>
-      </c>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49">
+        <v>389540.17</v>
+      </c>
+      <c r="J8" s="49"/>
     </row>
     <row r="9" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -3263,9 +3285,14 @@
       <c r="D9" s="3">
         <v>3</v>
       </c>
-      <c r="H9" s="5">
-        <v>361086.09</v>
-      </c>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49">
+        <v>389540.17</v>
+      </c>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
     </row>
     <row r="10" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -3280,9 +3307,14 @@
       <c r="D10" s="3">
         <v>4</v>
       </c>
-      <c r="G10" s="5">
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49">
         <v>2679.05</v>
       </c>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
     </row>
     <row r="11" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -3297,9 +3329,14 @@
       <c r="D11" s="3">
         <v>5</v>
       </c>
-      <c r="F11" s="5">
+      <c r="E11" s="49"/>
+      <c r="F11" s="49">
         <v>2679.05</v>
       </c>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
     </row>
     <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -3314,14 +3351,14 @@
       <c r="D12">
         <v>6</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="48">
         <v>2679.05</v>
       </c>
-      <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
     </row>
     <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -3336,9 +3373,14 @@
       <c r="D13" s="3">
         <v>4</v>
       </c>
-      <c r="G13" s="5">
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49">
         <v>183055.83</v>
       </c>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
     </row>
     <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -3353,9 +3395,14 @@
       <c r="D14" s="3">
         <v>5</v>
       </c>
-      <c r="F14" s="5">
+      <c r="E14" s="49"/>
+      <c r="F14" s="49">
         <v>178185.83</v>
       </c>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
     </row>
     <row r="15" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -3370,14 +3417,14 @@
       <c r="D15">
         <v>6</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="48">
         <v>178185.83</v>
       </c>
-      <c r="F15"/>
-      <c r="G15"/>
-      <c r="H15"/>
-      <c r="I15"/>
-      <c r="J15"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="48"/>
     </row>
     <row r="16" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -3392,9 +3439,14 @@
       <c r="D16" s="3">
         <v>5</v>
       </c>
-      <c r="F16" s="5">
+      <c r="E16" s="49"/>
+      <c r="F16" s="49">
         <v>4870</v>
       </c>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -3409,14 +3461,14 @@
       <c r="D17">
         <v>6</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="48">
         <v>0</v>
       </c>
-      <c r="F17"/>
-      <c r="G17"/>
-      <c r="H17"/>
-      <c r="I17"/>
-      <c r="J17"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
     </row>
     <row r="18" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -3431,14 +3483,14 @@
       <c r="D18">
         <v>6</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="48">
         <v>4870</v>
       </c>
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18"/>
-      <c r="I18"/>
-      <c r="J18"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="48"/>
     </row>
     <row r="19" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
@@ -3453,9 +3505,14 @@
       <c r="D19" s="3">
         <v>4</v>
       </c>
-      <c r="G19" s="5">
-        <v>114096.31</v>
-      </c>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49">
+        <v>142550.39000000001</v>
+      </c>
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
     </row>
     <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
@@ -3470,9 +3527,14 @@
       <c r="D20" s="3">
         <v>5</v>
       </c>
-      <c r="F20" s="5">
-        <v>114096.31</v>
-      </c>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49">
+        <v>142550.39000000001</v>
+      </c>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
     </row>
     <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -3487,14 +3549,14 @@
       <c r="D21">
         <v>6</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="48">
         <v>86113.69</v>
       </c>
-      <c r="F21"/>
-      <c r="G21"/>
-      <c r="H21"/>
-      <c r="I21"/>
-      <c r="J21"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
     </row>
     <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -3509,14 +3571,14 @@
       <c r="D22">
         <v>6</v>
       </c>
-      <c r="E22" s="2">
-        <v>27982.62</v>
-      </c>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
-      <c r="J22"/>
+      <c r="E22" s="48">
+        <v>56436.7</v>
+      </c>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
     </row>
     <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -3531,14 +3593,14 @@
       <c r="D23">
         <v>6</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="48">
         <v>0</v>
       </c>
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23"/>
-      <c r="I23"/>
-      <c r="J23"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="48"/>
     </row>
     <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -3553,14 +3615,14 @@
       <c r="D24">
         <v>6</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="48">
         <v>0</v>
       </c>
-      <c r="F24"/>
-      <c r="G24"/>
-      <c r="H24"/>
-      <c r="I24"/>
-      <c r="J24"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
     </row>
     <row r="25" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -3575,14 +3637,14 @@
       <c r="D25">
         <v>6</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="48">
         <v>0</v>
       </c>
-      <c r="F25"/>
-      <c r="G25"/>
-      <c r="H25"/>
-      <c r="I25"/>
-      <c r="J25"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="48"/>
     </row>
     <row r="26" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -3597,14 +3659,14 @@
       <c r="D26">
         <v>6</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="48">
         <v>0</v>
       </c>
-      <c r="F26"/>
-      <c r="G26"/>
-      <c r="H26"/>
-      <c r="I26"/>
-      <c r="J26"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="48"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="48"/>
     </row>
     <row r="27" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
@@ -3619,9 +3681,14 @@
       <c r="D27" s="3">
         <v>4</v>
       </c>
-      <c r="G27" s="5">
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49">
         <v>61254.9</v>
       </c>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="49"/>
     </row>
     <row r="28" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
@@ -3636,9 +3703,14 @@
       <c r="D28" s="3">
         <v>5</v>
       </c>
-      <c r="F28" s="5">
+      <c r="E28" s="49"/>
+      <c r="F28" s="49">
         <v>61254.9</v>
       </c>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
     </row>
     <row r="29" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29">
@@ -3653,14 +3725,14 @@
       <c r="D29">
         <v>6</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="48">
         <v>61056.94</v>
       </c>
-      <c r="F29"/>
-      <c r="G29"/>
-      <c r="H29"/>
-      <c r="I29"/>
-      <c r="J29"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="48"/>
+      <c r="H29" s="48"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="48"/>
     </row>
     <row r="30" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -3675,14 +3747,14 @@
       <c r="D30">
         <v>6</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="48">
         <v>197.96</v>
       </c>
-      <c r="F30"/>
-      <c r="G30"/>
-      <c r="H30"/>
-      <c r="I30"/>
-      <c r="J30"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="48"/>
     </row>
     <row r="31" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
@@ -3697,9 +3769,14 @@
       <c r="D31" s="3">
         <v>2</v>
       </c>
-      <c r="I31" s="5">
-        <v>221771.13</v>
-      </c>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="49">
+        <v>93444.75</v>
+      </c>
+      <c r="J31" s="49"/>
     </row>
     <row r="32" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
@@ -3714,9 +3791,14 @@
       <c r="D32" s="3">
         <v>3</v>
       </c>
-      <c r="H32" s="5">
-        <v>221771.13</v>
-      </c>
+      <c r="E32" s="49"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="49">
+        <v>93444.75</v>
+      </c>
+      <c r="I32" s="49"/>
+      <c r="J32" s="49"/>
     </row>
     <row r="33" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
@@ -3731,9 +3813,14 @@
       <c r="D33" s="3">
         <v>4</v>
       </c>
-      <c r="G33" s="5">
-        <v>190016.18</v>
-      </c>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="49">
+        <v>77559.710000000006</v>
+      </c>
+      <c r="H33" s="49"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="49"/>
     </row>
     <row r="34" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
@@ -3748,9 +3835,14 @@
       <c r="D34" s="3">
         <v>5</v>
       </c>
-      <c r="F34" s="5">
-        <v>190016.18</v>
-      </c>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49">
+        <v>77559.710000000006</v>
+      </c>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="49"/>
     </row>
     <row r="35" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35">
@@ -3765,1366 +3857,1491 @@
       <c r="D35">
         <v>6</v>
       </c>
-      <c r="E35" s="2">
-        <v>190016.18</v>
-      </c>
-      <c r="F35"/>
-      <c r="G35"/>
-      <c r="H35"/>
-      <c r="I35"/>
-      <c r="J35"/>
+      <c r="E35" s="48">
+        <v>77559.710000000006</v>
+      </c>
+      <c r="F35" s="48"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="48"/>
+      <c r="I35" s="48"/>
+      <c r="J35" s="48"/>
     </row>
     <row r="36" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
+      <c r="A36">
         <v>43</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D36" s="3">
-        <v>4</v>
-      </c>
-      <c r="G36" s="5">
-        <v>31754.95</v>
-      </c>
+      <c r="B36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36">
+        <v>6</v>
+      </c>
+      <c r="E36" s="48">
+        <v>0</v>
+      </c>
+      <c r="F36" s="48"/>
+      <c r="G36" s="48"/>
+      <c r="H36" s="48"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="48"/>
     </row>
     <row r="37" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D37" s="3">
+        <v>4</v>
+      </c>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49">
+        <v>15885.04</v>
+      </c>
+      <c r="H37" s="49"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="49"/>
+    </row>
+    <row r="38" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>46</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D38" s="3">
         <v>5</v>
       </c>
-      <c r="F37" s="5">
-        <v>31754.95</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>45</v>
-      </c>
-      <c r="B38" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D38">
-        <v>6</v>
-      </c>
-      <c r="E38" s="2">
-        <v>17354.150000000001</v>
-      </c>
-      <c r="F38"/>
-      <c r="G38"/>
-      <c r="H38"/>
-      <c r="I38"/>
-      <c r="J38"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49">
+        <v>15885.04</v>
+      </c>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="49"/>
+      <c r="J38" s="49"/>
     </row>
     <row r="39" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>47</v>
       </c>
       <c r="B39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39">
+        <v>6</v>
+      </c>
+      <c r="E39" s="48">
+        <v>1484.24</v>
+      </c>
+      <c r="F39" s="48"/>
+      <c r="G39" s="48"/>
+      <c r="H39" s="48"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
+    </row>
+    <row r="40" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>49</v>
+      </c>
+      <c r="B40" t="s">
         <v>72</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D39">
-        <v>6</v>
-      </c>
-      <c r="E39" s="2">
+      <c r="D40">
+        <v>6</v>
+      </c>
+      <c r="E40" s="48">
         <v>14400.8</v>
       </c>
-      <c r="F39"/>
-      <c r="G39"/>
-      <c r="H39"/>
-      <c r="I39"/>
-      <c r="J39"/>
-    </row>
-    <row r="40" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
-        <v>49</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D40" s="3">
-        <v>1</v>
-      </c>
-      <c r="J40" s="5">
-        <v>-1213.1300000000001</v>
-      </c>
+      <c r="F40" s="48"/>
+      <c r="G40" s="48"/>
+      <c r="H40" s="48"/>
+      <c r="I40" s="48"/>
+      <c r="J40" s="48"/>
     </row>
     <row r="41" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D41" s="3">
-        <v>2</v>
-      </c>
-      <c r="I41" s="5">
+        <v>1</v>
+      </c>
+      <c r="E41" s="49"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="49"/>
+      <c r="H41" s="49"/>
+      <c r="I41" s="49"/>
+      <c r="J41" s="49">
         <v>-1213.1300000000001</v>
       </c>
     </row>
     <row r="42" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D42" s="3">
-        <v>3</v>
-      </c>
-      <c r="H42" s="5">
+        <v>2</v>
+      </c>
+      <c r="E42" s="49"/>
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="49">
         <v>-1213.1300000000001</v>
       </c>
+      <c r="J42" s="49"/>
     </row>
     <row r="43" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D43" s="3">
-        <v>4</v>
-      </c>
-      <c r="G43" s="5">
+        <v>3</v>
+      </c>
+      <c r="E43" s="49"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="49">
         <v>-1213.1300000000001</v>
       </c>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49"/>
     </row>
     <row r="44" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" s="3">
+        <v>4</v>
+      </c>
+      <c r="E44" s="49"/>
+      <c r="F44" s="49"/>
+      <c r="G44" s="49">
+        <v>-1213.1300000000001</v>
+      </c>
+      <c r="H44" s="49"/>
+      <c r="I44" s="49"/>
+      <c r="J44" s="49"/>
+    </row>
+    <row r="45" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>55</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D45" s="3">
         <v>5</v>
       </c>
-      <c r="F44" s="3">
+      <c r="E45" s="49"/>
+      <c r="F45" s="49">
         <v>-704.57</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>54</v>
-      </c>
-      <c r="B45" t="s">
-        <v>84</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D45">
-        <v>6</v>
-      </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
-      <c r="F45"/>
-      <c r="G45"/>
-      <c r="H45"/>
-      <c r="I45"/>
-      <c r="J45"/>
+      <c r="G45" s="49"/>
+      <c r="H45" s="49"/>
+      <c r="I45" s="49"/>
+      <c r="J45" s="49"/>
     </row>
     <row r="46" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>56</v>
       </c>
       <c r="B46" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D46">
         <v>6</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="48">
         <v>0</v>
       </c>
-      <c r="F46"/>
-      <c r="G46"/>
-      <c r="H46"/>
-      <c r="I46"/>
-      <c r="J46"/>
+      <c r="F46" s="48"/>
+      <c r="G46" s="48"/>
+      <c r="H46" s="48"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="48"/>
     </row>
     <row r="47" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>58</v>
       </c>
       <c r="B47" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D47">
         <v>6</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="48">
         <v>0</v>
       </c>
-      <c r="F47"/>
-      <c r="G47"/>
-      <c r="H47"/>
-      <c r="I47"/>
-      <c r="J47"/>
+      <c r="F47" s="48"/>
+      <c r="G47" s="48"/>
+      <c r="H47" s="48"/>
+      <c r="I47" s="48"/>
+      <c r="J47" s="48"/>
     </row>
     <row r="48" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>60</v>
       </c>
       <c r="B48" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48">
+        <v>6</v>
+      </c>
+      <c r="E48" s="48">
+        <v>0</v>
+      </c>
+      <c r="F48" s="48"/>
+      <c r="G48" s="48"/>
+      <c r="H48" s="48"/>
+      <c r="I48" s="48"/>
+      <c r="J48" s="48"/>
+    </row>
+    <row r="49" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>62</v>
+      </c>
+      <c r="B49" t="s">
         <v>92</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D48">
-        <v>6</v>
-      </c>
-      <c r="E48">
+      <c r="D49">
+        <v>6</v>
+      </c>
+      <c r="E49" s="48">
         <v>-704.57</v>
       </c>
-      <c r="F48"/>
-      <c r="G48"/>
-      <c r="H48"/>
-      <c r="I48"/>
-      <c r="J48"/>
-    </row>
-    <row r="49" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3">
-        <v>62</v>
-      </c>
-      <c r="B49" s="3" t="s">
+      <c r="F49" s="48"/>
+      <c r="G49" s="48"/>
+      <c r="H49" s="48"/>
+      <c r="I49" s="48"/>
+      <c r="J49" s="48"/>
+    </row>
+    <row r="50" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>64</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C50" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D50" s="3">
         <v>5</v>
       </c>
-      <c r="F49" s="3">
+      <c r="E50" s="49"/>
+      <c r="F50" s="49">
         <v>-508.56</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>63</v>
-      </c>
-      <c r="B50" t="s">
-        <v>98</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D50">
-        <v>6</v>
-      </c>
-      <c r="E50">
-        <v>0</v>
-      </c>
-      <c r="F50"/>
-      <c r="G50"/>
-      <c r="H50"/>
-      <c r="I50"/>
-      <c r="J50"/>
+      <c r="G50" s="49"/>
+      <c r="H50" s="49"/>
+      <c r="I50" s="49"/>
+      <c r="J50" s="49"/>
     </row>
     <row r="51" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>65</v>
       </c>
       <c r="B51" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D51">
         <v>6</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="48">
         <v>0</v>
       </c>
-      <c r="F51"/>
-      <c r="G51"/>
-      <c r="H51"/>
-      <c r="I51"/>
-      <c r="J51"/>
+      <c r="F51" s="48"/>
+      <c r="G51" s="48"/>
+      <c r="H51" s="48"/>
+      <c r="I51" s="48"/>
+      <c r="J51" s="48"/>
     </row>
     <row r="52" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>67</v>
       </c>
       <c r="B52" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D52">
         <v>6</v>
       </c>
-      <c r="E52">
-        <v>-508.56</v>
-      </c>
-      <c r="F52"/>
-      <c r="G52"/>
-      <c r="H52"/>
-      <c r="I52"/>
-      <c r="J52"/>
+      <c r="E52" s="48">
+        <v>0</v>
+      </c>
+      <c r="F52" s="48"/>
+      <c r="G52" s="48"/>
+      <c r="H52" s="48"/>
+      <c r="I52" s="48"/>
+      <c r="J52" s="48"/>
     </row>
     <row r="53" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>69</v>
       </c>
       <c r="B53" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D53">
+        <v>6</v>
+      </c>
+      <c r="E53" s="48">
+        <v>-508.56</v>
+      </c>
+      <c r="F53" s="48"/>
+      <c r="G53" s="48"/>
+      <c r="H53" s="48"/>
+      <c r="I53" s="48"/>
+      <c r="J53" s="48"/>
+    </row>
+    <row r="54" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>71</v>
+      </c>
+      <c r="B54" t="s">
         <v>427</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="D53">
-        <v>6</v>
-      </c>
-      <c r="E53">
+      <c r="D54">
+        <v>6</v>
+      </c>
+      <c r="E54" s="48">
         <v>0</v>
       </c>
-      <c r="F53"/>
-      <c r="G53"/>
-      <c r="H53"/>
-      <c r="I53"/>
-      <c r="J53"/>
-    </row>
-    <row r="54" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="3">
-        <v>71</v>
-      </c>
-      <c r="B54" s="3" t="s">
+      <c r="F54" s="48"/>
+      <c r="G54" s="48"/>
+      <c r="H54" s="48"/>
+      <c r="I54" s="48"/>
+      <c r="J54" s="48"/>
+    </row>
+    <row r="55" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <v>73</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C55" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D55" s="3">
         <v>5</v>
       </c>
-      <c r="F54" s="3">
+      <c r="E55" s="49"/>
+      <c r="F55" s="49">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>72</v>
-      </c>
-      <c r="B55" t="s">
+      <c r="G55" s="49"/>
+      <c r="H55" s="49"/>
+      <c r="I55" s="49"/>
+      <c r="J55" s="49"/>
+    </row>
+    <row r="56" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>74</v>
+      </c>
+      <c r="B56" t="s">
         <v>106</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D55">
-        <v>6</v>
-      </c>
-      <c r="E55">
+      <c r="D56">
+        <v>6</v>
+      </c>
+      <c r="E56" s="48">
         <v>0</v>
       </c>
-      <c r="F55"/>
-      <c r="G55"/>
-      <c r="H55"/>
-      <c r="I55"/>
-      <c r="J55"/>
-    </row>
-    <row r="56" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="3">
-        <v>74</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D56" s="3">
-        <v>4</v>
-      </c>
-      <c r="G56" s="3">
-        <v>0</v>
-      </c>
+      <c r="F56" s="48"/>
+      <c r="G56" s="48"/>
+      <c r="H56" s="48"/>
+      <c r="I56" s="48"/>
+      <c r="J56" s="48"/>
     </row>
     <row r="57" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B57" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D57" s="3">
+        <v>4</v>
+      </c>
+      <c r="E57" s="49"/>
+      <c r="F57" s="49"/>
+      <c r="G57" s="49">
+        <v>0</v>
+      </c>
+      <c r="H57" s="49"/>
+      <c r="I57" s="49"/>
+      <c r="J57" s="49"/>
+    </row>
+    <row r="58" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <v>77</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C58" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D57" s="3">
+      <c r="D58" s="3">
         <v>5</v>
       </c>
-      <c r="F57" s="3">
+      <c r="E58" s="49"/>
+      <c r="F58" s="49">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>76</v>
-      </c>
-      <c r="B58" t="s">
+      <c r="G58" s="49"/>
+      <c r="H58" s="49"/>
+      <c r="I58" s="49"/>
+      <c r="J58" s="49"/>
+    </row>
+    <row r="59" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>78</v>
+      </c>
+      <c r="B59" t="s">
         <v>112</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D58">
-        <v>6</v>
-      </c>
-      <c r="E58">
+      <c r="D59">
+        <v>6</v>
+      </c>
+      <c r="E59" s="48">
         <v>0</v>
       </c>
-      <c r="F58"/>
-      <c r="G58"/>
-      <c r="H58"/>
-      <c r="I58"/>
-      <c r="J58"/>
-    </row>
-    <row r="59" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="3">
-        <v>78</v>
-      </c>
-      <c r="B59" s="3" t="s">
+      <c r="F59" s="48"/>
+      <c r="G59" s="48"/>
+      <c r="H59" s="48"/>
+      <c r="I59" s="48"/>
+      <c r="J59" s="48"/>
+    </row>
+    <row r="60" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
+        <v>80</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C60" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D59" s="3">
+      <c r="D60" s="3">
         <v>5</v>
       </c>
-      <c r="F59" s="3">
+      <c r="E60" s="49"/>
+      <c r="F60" s="49">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>79</v>
-      </c>
-      <c r="B60" t="s">
+      <c r="G60" s="49"/>
+      <c r="H60" s="49"/>
+      <c r="I60" s="49"/>
+      <c r="J60" s="49"/>
+    </row>
+    <row r="61" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>81</v>
+      </c>
+      <c r="B61" t="s">
         <v>116</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D60">
-        <v>6</v>
-      </c>
-      <c r="E60">
+      <c r="D61">
+        <v>6</v>
+      </c>
+      <c r="E61" s="48">
         <v>0</v>
       </c>
-      <c r="F60"/>
-      <c r="G60"/>
-      <c r="H60"/>
-      <c r="I60"/>
-      <c r="J60"/>
-    </row>
-    <row r="61" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="3">
-        <v>81</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D61" s="3">
-        <v>4</v>
-      </c>
-      <c r="G61" s="3">
-        <v>0</v>
-      </c>
+      <c r="F61" s="48"/>
+      <c r="G61" s="48"/>
+      <c r="H61" s="48"/>
+      <c r="I61" s="48"/>
+      <c r="J61" s="48"/>
     </row>
     <row r="62" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B62" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D62" s="3">
+        <v>4</v>
+      </c>
+      <c r="E62" s="49"/>
+      <c r="F62" s="49"/>
+      <c r="G62" s="49">
+        <v>0</v>
+      </c>
+      <c r="H62" s="49"/>
+      <c r="I62" s="49"/>
+      <c r="J62" s="49"/>
+    </row>
+    <row r="63" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
+        <v>84</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C63" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D62" s="3">
+      <c r="D63" s="3">
         <v>5</v>
       </c>
-      <c r="F62" s="3">
+      <c r="E63" s="49"/>
+      <c r="F63" s="49">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>83</v>
-      </c>
-      <c r="B63" t="s">
+      <c r="G63" s="49"/>
+      <c r="H63" s="49"/>
+      <c r="I63" s="49"/>
+      <c r="J63" s="49"/>
+    </row>
+    <row r="64" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>85</v>
+      </c>
+      <c r="B64" t="s">
         <v>122</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D63">
-        <v>6</v>
-      </c>
-      <c r="E63">
+      <c r="D64">
+        <v>6</v>
+      </c>
+      <c r="E64" s="48">
         <v>0</v>
       </c>
-      <c r="F63"/>
-      <c r="G63"/>
-      <c r="H63"/>
-      <c r="I63"/>
-      <c r="J63"/>
-    </row>
-    <row r="64" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="3">
-        <v>85</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D64" s="3">
-        <v>4</v>
-      </c>
-      <c r="G64" s="3">
-        <v>0</v>
-      </c>
+      <c r="F64" s="48"/>
+      <c r="G64" s="48"/>
+      <c r="H64" s="48"/>
+      <c r="I64" s="48"/>
+      <c r="J64" s="48"/>
     </row>
     <row r="65" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B65" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D65" s="3">
+        <v>4</v>
+      </c>
+      <c r="E65" s="49"/>
+      <c r="F65" s="49"/>
+      <c r="G65" s="49">
+        <v>0</v>
+      </c>
+      <c r="H65" s="49"/>
+      <c r="I65" s="49"/>
+      <c r="J65" s="49"/>
+    </row>
+    <row r="66" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3">
+        <v>88</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C66" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D65" s="3">
+      <c r="D66" s="3">
         <v>5</v>
       </c>
-      <c r="F65" s="3">
+      <c r="E66" s="49"/>
+      <c r="F66" s="49">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>87</v>
-      </c>
-      <c r="B66" t="s">
+      <c r="G66" s="49"/>
+      <c r="H66" s="49"/>
+      <c r="I66" s="49"/>
+      <c r="J66" s="49"/>
+    </row>
+    <row r="67" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>89</v>
+      </c>
+      <c r="B67" t="s">
         <v>128</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D66">
-        <v>6</v>
-      </c>
-      <c r="E66">
+      <c r="D67">
+        <v>6</v>
+      </c>
+      <c r="E67" s="48">
         <v>0</v>
       </c>
-      <c r="F66"/>
-      <c r="G66"/>
-      <c r="H66"/>
-      <c r="I66"/>
-      <c r="J66"/>
-    </row>
-    <row r="67" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="3">
-        <v>89</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D67" s="3">
-        <v>1</v>
-      </c>
-      <c r="J67" s="5">
-        <v>-428311.39</v>
-      </c>
+      <c r="F67" s="48"/>
+      <c r="G67" s="48"/>
+      <c r="H67" s="48"/>
+      <c r="I67" s="48"/>
+      <c r="J67" s="48"/>
     </row>
     <row r="68" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D68" s="3">
-        <v>2</v>
-      </c>
-      <c r="I68" s="5">
-        <v>-20000</v>
+        <v>1</v>
+      </c>
+      <c r="E68" s="49"/>
+      <c r="F68" s="49"/>
+      <c r="G68" s="49"/>
+      <c r="H68" s="49"/>
+      <c r="I68" s="49"/>
+      <c r="J68" s="49">
+        <v>-428311.39</v>
       </c>
     </row>
     <row r="69" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D69" s="3">
-        <v>3</v>
-      </c>
-      <c r="H69" s="5">
+        <v>2</v>
+      </c>
+      <c r="E69" s="49"/>
+      <c r="F69" s="49"/>
+      <c r="G69" s="49"/>
+      <c r="H69" s="49"/>
+      <c r="I69" s="49">
         <v>-20000</v>
       </c>
+      <c r="J69" s="49"/>
     </row>
     <row r="70" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D70" s="3">
-        <v>4</v>
-      </c>
-      <c r="G70" s="5">
+        <v>3</v>
+      </c>
+      <c r="E70" s="49"/>
+      <c r="F70" s="49"/>
+      <c r="G70" s="49"/>
+      <c r="H70" s="49">
         <v>-20000</v>
       </c>
+      <c r="I70" s="49"/>
+      <c r="J70" s="49"/>
     </row>
     <row r="71" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B71" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D71" s="3">
+        <v>4</v>
+      </c>
+      <c r="E71" s="49"/>
+      <c r="F71" s="49"/>
+      <c r="G71" s="49">
+        <v>-20000</v>
+      </c>
+      <c r="H71" s="49"/>
+      <c r="I71" s="49"/>
+      <c r="J71" s="49"/>
+    </row>
+    <row r="72" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3">
+        <v>95</v>
+      </c>
+      <c r="B72" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C72" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D71" s="3">
+      <c r="D72" s="3">
         <v>5</v>
       </c>
-      <c r="F71" s="5">
+      <c r="E72" s="49"/>
+      <c r="F72" s="49">
         <v>-20000</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>94</v>
-      </c>
-      <c r="B72" t="s">
+      <c r="G72" s="49"/>
+      <c r="H72" s="49"/>
+      <c r="I72" s="49"/>
+      <c r="J72" s="49"/>
+    </row>
+    <row r="73" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>96</v>
+      </c>
+      <c r="B73" t="s">
         <v>140</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C73" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D72">
-        <v>6</v>
-      </c>
-      <c r="E72" s="2">
+      <c r="D73">
+        <v>6</v>
+      </c>
+      <c r="E73" s="48">
         <v>-20000</v>
       </c>
-      <c r="F72"/>
-      <c r="G72"/>
-      <c r="H72"/>
-      <c r="I72"/>
-      <c r="J72"/>
-    </row>
-    <row r="73" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="3">
-        <v>96</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D73" s="3">
-        <v>2</v>
-      </c>
-      <c r="I73" s="5">
-        <v>-346584.46</v>
-      </c>
+      <c r="F73" s="48"/>
+      <c r="G73" s="48"/>
+      <c r="H73" s="48"/>
+      <c r="I73" s="48"/>
+      <c r="J73" s="48"/>
     </row>
     <row r="74" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D74" s="3">
-        <v>3</v>
-      </c>
-      <c r="H74" s="5">
+        <v>2</v>
+      </c>
+      <c r="E74" s="49"/>
+      <c r="F74" s="49"/>
+      <c r="G74" s="49"/>
+      <c r="H74" s="49"/>
+      <c r="I74" s="49">
         <v>-346584.46</v>
       </c>
+      <c r="J74" s="49"/>
     </row>
     <row r="75" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D75" s="3">
-        <v>4</v>
-      </c>
-      <c r="G75" s="5">
+        <v>3</v>
+      </c>
+      <c r="E75" s="49"/>
+      <c r="F75" s="49"/>
+      <c r="G75" s="49"/>
+      <c r="H75" s="49">
         <v>-346584.46</v>
       </c>
+      <c r="I75" s="49"/>
+      <c r="J75" s="49"/>
     </row>
     <row r="76" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B76" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D76" s="3">
+        <v>4</v>
+      </c>
+      <c r="E76" s="49"/>
+      <c r="F76" s="49"/>
+      <c r="G76" s="49">
+        <v>-346584.46</v>
+      </c>
+      <c r="H76" s="49"/>
+      <c r="I76" s="49"/>
+      <c r="J76" s="49"/>
+    </row>
+    <row r="77" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3">
+        <v>101</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C76" s="4" t="s">
+      <c r="C77" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D76" s="3">
+      <c r="D77" s="3">
         <v>5</v>
       </c>
-      <c r="F76" s="5">
+      <c r="E77" s="49"/>
+      <c r="F77" s="49">
         <v>-346584.46</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>100</v>
-      </c>
-      <c r="B77" t="s">
-        <v>150</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D77">
-        <v>6</v>
-      </c>
-      <c r="E77" s="2">
-        <v>-142203.51</v>
-      </c>
-      <c r="F77"/>
-      <c r="G77"/>
-      <c r="H77"/>
-      <c r="I77"/>
-      <c r="J77"/>
+      <c r="G77" s="49"/>
+      <c r="H77" s="49"/>
+      <c r="I77" s="49"/>
+      <c r="J77" s="49"/>
     </row>
     <row r="78" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>102</v>
       </c>
       <c r="B78" t="s">
+        <v>150</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D78">
+        <v>6</v>
+      </c>
+      <c r="E78" s="48">
+        <v>-142203.51</v>
+      </c>
+      <c r="F78" s="48"/>
+      <c r="G78" s="48"/>
+      <c r="H78" s="48"/>
+      <c r="I78" s="48"/>
+      <c r="J78" s="48"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>104</v>
+      </c>
+      <c r="B79" t="s">
         <v>152</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D78">
-        <v>6</v>
-      </c>
-      <c r="E78" s="2">
+      <c r="D79">
+        <v>6</v>
+      </c>
+      <c r="E79" s="48">
         <v>-204380.95</v>
       </c>
-      <c r="F78"/>
-      <c r="G78"/>
-      <c r="H78"/>
-      <c r="I78"/>
-      <c r="J78"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="3">
-        <v>104</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D79" s="3">
-        <v>2</v>
-      </c>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
-      <c r="G79" s="3"/>
-      <c r="H79" s="3"/>
-      <c r="I79" s="5">
-        <v>-61726.93</v>
-      </c>
-      <c r="J79" s="3"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D80" s="3">
-        <v>3</v>
-      </c>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
-      <c r="G80" s="3"/>
-      <c r="H80" s="5">
+        <v>2</v>
+      </c>
+      <c r="E80" s="49"/>
+      <c r="F80" s="49"/>
+      <c r="G80" s="49"/>
+      <c r="H80" s="49"/>
+      <c r="I80" s="49">
         <v>-61726.93</v>
       </c>
-      <c r="I80" s="3"/>
-      <c r="J80" s="3"/>
+      <c r="J80" s="49"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D81" s="3">
-        <v>4</v>
-      </c>
-      <c r="E81" s="3"/>
-      <c r="F81" s="3"/>
-      <c r="G81" s="5">
+        <v>3</v>
+      </c>
+      <c r="E81" s="49"/>
+      <c r="F81" s="49"/>
+      <c r="G81" s="49"/>
+      <c r="H81" s="49">
         <v>-61726.93</v>
       </c>
-      <c r="H81" s="3"/>
-      <c r="I81" s="3"/>
-      <c r="J81" s="3"/>
+      <c r="I81" s="49"/>
+      <c r="J81" s="49"/>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B82" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D82" s="3">
+        <v>4</v>
+      </c>
+      <c r="E82" s="49"/>
+      <c r="F82" s="49"/>
+      <c r="G82" s="49">
+        <v>-61726.93</v>
+      </c>
+      <c r="H82" s="49"/>
+      <c r="I82" s="49"/>
+      <c r="J82" s="49"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="3">
+        <v>109</v>
+      </c>
+      <c r="B83" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C82" s="4" t="s">
+      <c r="C83" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D82" s="3">
+      <c r="D83" s="3">
         <v>5</v>
       </c>
-      <c r="E82" s="3"/>
-      <c r="F82" s="5">
+      <c r="E83" s="49"/>
+      <c r="F83" s="49">
         <v>-61726.93</v>
       </c>
-      <c r="G82" s="3"/>
-      <c r="H82" s="3"/>
-      <c r="I82" s="3"/>
-      <c r="J82" s="3"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>108</v>
-      </c>
-      <c r="B83" t="s">
+      <c r="G83" s="49"/>
+      <c r="H83" s="49"/>
+      <c r="I83" s="49"/>
+      <c r="J83" s="49"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>110</v>
+      </c>
+      <c r="B84" t="s">
         <v>162</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D83">
-        <v>6</v>
-      </c>
-      <c r="E83" s="2">
+      <c r="D84">
+        <v>6</v>
+      </c>
+      <c r="E84" s="48">
         <v>-61726.93</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B84" s="3"/>
-    </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B85" s="7" t="s">
+      <c r="C85" s="1"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B86" s="7" t="s">
         <v>429</v>
       </c>
-      <c r="C85" s="7"/>
-      <c r="D85" s="7"/>
-      <c r="E85" s="7"/>
-      <c r="F85" s="7"/>
-      <c r="G85" s="7"/>
-      <c r="H85" s="7"/>
-      <c r="I85" s="7"/>
-      <c r="J85" s="8">
-        <f>+J132</f>
-        <v>-153332.70000000001</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B87" s="42" t="s">
+      <c r="C86" s="7"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="50"/>
+      <c r="F86" s="50"/>
+      <c r="G86" s="50"/>
+      <c r="H86" s="50"/>
+      <c r="I86" s="50"/>
+      <c r="J86" s="50">
+        <f>+J133</f>
+        <v>-53460.399999999994</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B88" s="42" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
         <v>424</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="3">
-        <v>110</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C90" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="D90" s="3">
-        <v>1</v>
-      </c>
-      <c r="E90" s="3"/>
-      <c r="F90" s="3"/>
-      <c r="G90" s="3"/>
-      <c r="H90" s="3"/>
-      <c r="I90" s="3"/>
-      <c r="J90" s="5">
-        <v>-547020</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D91" s="3">
-        <v>2</v>
-      </c>
-      <c r="E91" s="3"/>
-      <c r="F91" s="3"/>
-      <c r="G91" s="3"/>
-      <c r="H91" s="3"/>
-      <c r="I91" s="5">
+        <v>1</v>
+      </c>
+      <c r="E91" s="49"/>
+      <c r="F91" s="49"/>
+      <c r="G91" s="49"/>
+      <c r="H91" s="49"/>
+      <c r="I91" s="49"/>
+      <c r="J91" s="49">
         <v>-547020</v>
       </c>
-      <c r="J91" s="3"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D92" s="3">
-        <v>3</v>
-      </c>
-      <c r="E92" s="3"/>
-      <c r="F92" s="3"/>
-      <c r="G92" s="3"/>
-      <c r="H92" s="5">
+        <v>2</v>
+      </c>
+      <c r="E92" s="49"/>
+      <c r="F92" s="49"/>
+      <c r="G92" s="49"/>
+      <c r="H92" s="49"/>
+      <c r="I92" s="49">
         <v>-547020</v>
       </c>
-      <c r="I92" s="3"/>
-      <c r="J92" s="3"/>
+      <c r="J92" s="49"/>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D93" s="3">
-        <v>4</v>
-      </c>
-      <c r="E93" s="3"/>
-      <c r="F93" s="3"/>
-      <c r="G93" s="5">
+        <v>3</v>
+      </c>
+      <c r="E93" s="49"/>
+      <c r="F93" s="49"/>
+      <c r="G93" s="49"/>
+      <c r="H93" s="49">
         <v>-547020</v>
       </c>
-      <c r="H93" s="3"/>
-      <c r="I93" s="3"/>
-      <c r="J93" s="3"/>
+      <c r="I93" s="49"/>
+      <c r="J93" s="49"/>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B94" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D94" s="3">
+        <v>4</v>
+      </c>
+      <c r="E94" s="49"/>
+      <c r="F94" s="49"/>
+      <c r="G94" s="49">
+        <v>-547020</v>
+      </c>
+      <c r="H94" s="49"/>
+      <c r="I94" s="49"/>
+      <c r="J94" s="49"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="3">
+        <v>116</v>
+      </c>
+      <c r="B95" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C94" s="4" t="s">
+      <c r="C95" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D94" s="3">
+      <c r="D95" s="3">
         <v>5</v>
       </c>
-      <c r="E94" s="3"/>
-      <c r="F94" s="5">
+      <c r="E95" s="49"/>
+      <c r="F95" s="49">
         <v>-547020</v>
       </c>
-      <c r="G94" s="3"/>
-      <c r="H94" s="3"/>
-      <c r="I94" s="3"/>
-      <c r="J94" s="3"/>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>115</v>
-      </c>
-      <c r="B95" t="s">
+      <c r="G95" s="49"/>
+      <c r="H95" s="49"/>
+      <c r="I95" s="49"/>
+      <c r="J95" s="49"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>117</v>
+      </c>
+      <c r="B96" t="s">
         <v>176</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C96" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="D95">
-        <v>6</v>
-      </c>
-      <c r="E95" s="2">
+      <c r="D96">
+        <v>6</v>
+      </c>
+      <c r="E96" s="48">
         <v>-547020</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" s="3">
-        <v>117</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C96" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="D96" s="3">
-        <v>1</v>
-      </c>
-      <c r="E96" s="3"/>
-      <c r="F96" s="3"/>
-      <c r="G96" s="3"/>
-      <c r="H96" s="3"/>
-      <c r="I96" s="3"/>
-      <c r="J96" s="5">
-        <v>264271.33</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D97" s="3">
-        <v>2</v>
-      </c>
-      <c r="E97" s="3"/>
-      <c r="F97" s="3"/>
-      <c r="G97" s="3"/>
-      <c r="H97" s="3"/>
-      <c r="I97" s="5">
-        <v>264271.33</v>
-      </c>
-      <c r="J97" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="E97" s="49"/>
+      <c r="F97" s="49"/>
+      <c r="G97" s="49"/>
+      <c r="H97" s="49"/>
+      <c r="I97" s="49"/>
+      <c r="J97" s="49">
+        <v>392066.26</v>
+      </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D98" s="3">
-        <v>3</v>
-      </c>
-      <c r="E98" s="3"/>
-      <c r="F98" s="3"/>
-      <c r="G98" s="3"/>
-      <c r="H98" s="5">
-        <v>264271.33</v>
-      </c>
-      <c r="I98" s="3"/>
-      <c r="J98" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="E98" s="49"/>
+      <c r="F98" s="49"/>
+      <c r="G98" s="49"/>
+      <c r="H98" s="49"/>
+      <c r="I98" s="49">
+        <v>392066.26</v>
+      </c>
+      <c r="J98" s="49"/>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D99" s="3">
-        <v>4</v>
-      </c>
-      <c r="E99" s="3"/>
-      <c r="F99" s="3"/>
-      <c r="G99" s="5">
-        <v>264271.33</v>
-      </c>
-      <c r="H99" s="3"/>
-      <c r="I99" s="3"/>
-      <c r="J99" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="E99" s="49"/>
+      <c r="F99" s="49"/>
+      <c r="G99" s="49"/>
+      <c r="H99" s="49">
+        <v>392066.26</v>
+      </c>
+      <c r="I99" s="49"/>
+      <c r="J99" s="49"/>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B100" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D100" s="3">
+        <v>4</v>
+      </c>
+      <c r="E100" s="49"/>
+      <c r="F100" s="49"/>
+      <c r="G100" s="49">
+        <v>392066.26</v>
+      </c>
+      <c r="H100" s="49"/>
+      <c r="I100" s="49"/>
+      <c r="J100" s="49"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="3">
+        <v>123</v>
+      </c>
+      <c r="B101" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="C100" s="4" t="s">
+      <c r="C101" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="D100" s="3">
+      <c r="D101" s="3">
         <v>5</v>
       </c>
-      <c r="E100" s="3"/>
-      <c r="F100" s="5">
-        <v>264271.33</v>
-      </c>
-      <c r="G100" s="3"/>
-      <c r="H100" s="3"/>
-      <c r="I100" s="3"/>
-      <c r="J100" s="3"/>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101">
-        <v>122</v>
-      </c>
-      <c r="B101" t="s">
+      <c r="E101" s="49"/>
+      <c r="F101" s="49">
+        <v>392066.26</v>
+      </c>
+      <c r="G101" s="49"/>
+      <c r="H101" s="49"/>
+      <c r="I101" s="49"/>
+      <c r="J101" s="49"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>124</v>
+      </c>
+      <c r="B102" t="s">
         <v>188</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C102" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="D101">
-        <v>6</v>
-      </c>
-      <c r="E101" s="2">
-        <v>264271.33</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" s="3">
-        <v>124</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="C102" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="D102" s="3">
-        <v>1</v>
-      </c>
-      <c r="E102" s="3"/>
-      <c r="F102" s="3"/>
-      <c r="G102" s="3"/>
-      <c r="H102" s="3"/>
-      <c r="I102" s="3"/>
-      <c r="J102" s="5">
-        <v>128405.61</v>
+      <c r="D102">
+        <v>6</v>
+      </c>
+      <c r="E102" s="48">
+        <v>392066.26</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D103" s="3">
-        <v>2</v>
-      </c>
-      <c r="E103" s="3"/>
-      <c r="F103" s="3"/>
-      <c r="G103" s="3"/>
-      <c r="H103" s="3"/>
-      <c r="I103" s="5">
-        <v>128405.61</v>
-      </c>
-      <c r="J103" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="E103" s="49"/>
+      <c r="F103" s="49"/>
+      <c r="G103" s="49"/>
+      <c r="H103" s="49"/>
+      <c r="I103" s="49"/>
+      <c r="J103" s="49">
+        <v>100482.98</v>
+      </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D104" s="3">
-        <v>3</v>
-      </c>
-      <c r="E104" s="3"/>
-      <c r="F104" s="3"/>
-      <c r="G104" s="3"/>
-      <c r="H104" s="5">
-        <v>128351.97</v>
-      </c>
-      <c r="I104" s="3"/>
-      <c r="J104" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="E104" s="49"/>
+      <c r="F104" s="49"/>
+      <c r="G104" s="49"/>
+      <c r="H104" s="49"/>
+      <c r="I104" s="49">
+        <v>100482.98</v>
+      </c>
+      <c r="J104" s="49"/>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D105" s="3">
-        <v>4</v>
-      </c>
-      <c r="E105" s="3"/>
-      <c r="F105" s="3"/>
-      <c r="G105" s="5">
-        <v>128351.97</v>
-      </c>
-      <c r="H105" s="3"/>
-      <c r="I105" s="3"/>
-      <c r="J105" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="E105" s="49"/>
+      <c r="F105" s="49"/>
+      <c r="G105" s="49"/>
+      <c r="H105" s="49">
+        <v>100429.34</v>
+      </c>
+      <c r="I105" s="49"/>
+      <c r="J105" s="49"/>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B106" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D106" s="3">
+        <v>4</v>
+      </c>
+      <c r="E106" s="49"/>
+      <c r="F106" s="49"/>
+      <c r="G106" s="49">
+        <v>100429.34</v>
+      </c>
+      <c r="H106" s="49"/>
+      <c r="I106" s="49"/>
+      <c r="J106" s="49"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="3">
+        <v>130</v>
+      </c>
+      <c r="B107" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="C106" s="4" t="s">
+      <c r="C107" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="D106" s="3">
+      <c r="D107" s="3">
         <v>5</v>
       </c>
-      <c r="E106" s="3"/>
-      <c r="F106" s="5">
-        <v>128351.97</v>
-      </c>
-      <c r="G106" s="3"/>
-      <c r="H106" s="3"/>
-      <c r="I106" s="3"/>
-      <c r="J106" s="3"/>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A107">
-        <v>129</v>
-      </c>
-      <c r="B107" t="s">
-        <v>220</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="D107">
-        <v>6</v>
-      </c>
-      <c r="E107">
-        <v>20.52</v>
-      </c>
+      <c r="E107" s="49"/>
+      <c r="F107" s="49">
+        <v>100429.34</v>
+      </c>
+      <c r="G107" s="49"/>
+      <c r="H107" s="49"/>
+      <c r="I107" s="49"/>
+      <c r="J107" s="49"/>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>131</v>
       </c>
       <c r="B108" t="s">
-        <v>432</v>
+        <v>220</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D108">
         <v>6</v>
       </c>
-      <c r="E108">
-        <v>0</v>
+      <c r="E108" s="48">
+        <v>20.52</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
@@ -5132,16 +5349,16 @@
         <v>133</v>
       </c>
       <c r="B109" t="s">
-        <v>200</v>
+        <v>432</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>201</v>
+        <v>433</v>
       </c>
       <c r="D109">
         <v>6</v>
       </c>
-      <c r="E109" s="2">
-        <v>2311.25</v>
+      <c r="E109" s="48">
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
@@ -5149,16 +5366,16 @@
         <v>135</v>
       </c>
       <c r="B110" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="D110">
         <v>6</v>
       </c>
-      <c r="E110">
-        <v>0</v>
+      <c r="E110" s="48">
+        <v>2842.7</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
@@ -5166,16 +5383,16 @@
         <v>137</v>
       </c>
       <c r="B111" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D111">
         <v>6</v>
       </c>
-      <c r="E111" s="2">
-        <v>78754.399999999994</v>
+      <c r="E111" s="48">
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
@@ -5183,16 +5400,16 @@
         <v>139</v>
       </c>
       <c r="B112" t="s">
-        <v>434</v>
+        <v>208</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>402</v>
+        <v>209</v>
       </c>
       <c r="D112">
         <v>6</v>
       </c>
-      <c r="E112">
-        <v>22</v>
+      <c r="E112" s="48">
+        <v>78754.399999999994</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
@@ -5200,16 +5417,16 @@
         <v>141</v>
       </c>
       <c r="B113" t="s">
-        <v>210</v>
+        <v>434</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>211</v>
+        <v>402</v>
       </c>
       <c r="D113">
         <v>6</v>
       </c>
-      <c r="E113" s="2">
-        <v>3245.59</v>
+      <c r="E113" s="48">
+        <v>22</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
@@ -5217,16 +5434,16 @@
         <v>143</v>
       </c>
       <c r="B114" t="s">
-        <v>435</v>
+        <v>210</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>436</v>
+        <v>211</v>
       </c>
       <c r="D114">
         <v>6</v>
       </c>
-      <c r="E114">
-        <v>154.1</v>
+      <c r="E114" s="48">
+        <v>3245.59</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
@@ -5234,351 +5451,367 @@
         <v>145</v>
       </c>
       <c r="B115" t="s">
+        <v>435</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D115">
+        <v>6</v>
+      </c>
+      <c r="E115" s="48">
+        <v>154.1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>147</v>
+      </c>
+      <c r="B116" t="s">
         <v>212</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="C116" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="D115">
-        <v>6</v>
-      </c>
-      <c r="E115" s="2">
-        <v>43844.11</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A116" s="3">
-        <v>147</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="C116" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="D116" s="3">
-        <v>3</v>
-      </c>
-      <c r="E116" s="3"/>
-      <c r="F116" s="3"/>
-      <c r="G116" s="3"/>
-      <c r="H116" s="3">
-        <v>53.64</v>
-      </c>
-      <c r="I116" s="3"/>
-      <c r="J116" s="3"/>
+      <c r="D116">
+        <v>6</v>
+      </c>
+      <c r="E116" s="48">
+        <v>15390.03</v>
+      </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D117" s="3">
-        <v>4</v>
-      </c>
-      <c r="E117" s="3"/>
-      <c r="F117" s="3"/>
-      <c r="G117" s="3">
+        <v>3</v>
+      </c>
+      <c r="E117" s="49"/>
+      <c r="F117" s="49"/>
+      <c r="G117" s="49"/>
+      <c r="H117" s="49">
         <v>53.64</v>
       </c>
-      <c r="H117" s="3"/>
-      <c r="I117" s="3"/>
-      <c r="J117" s="3"/>
+      <c r="I117" s="49"/>
+      <c r="J117" s="49"/>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B118" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C118" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="D118" s="3">
+        <v>4</v>
+      </c>
+      <c r="E118" s="49"/>
+      <c r="F118" s="49"/>
+      <c r="G118" s="49">
+        <v>53.64</v>
+      </c>
+      <c r="H118" s="49"/>
+      <c r="I118" s="49"/>
+      <c r="J118" s="49"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A119" s="3">
+        <v>151</v>
+      </c>
+      <c r="B119" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="C118" s="4" t="s">
+      <c r="C119" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="D118" s="3">
+      <c r="D119" s="3">
         <v>5</v>
       </c>
-      <c r="E118" s="3"/>
-      <c r="F118" s="3">
+      <c r="E119" s="49"/>
+      <c r="F119" s="49">
         <v>53.64</v>
       </c>
-      <c r="G118" s="3"/>
-      <c r="H118" s="3"/>
-      <c r="I118" s="3"/>
-      <c r="J118" s="3"/>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A119">
-        <v>150</v>
-      </c>
-      <c r="B119" t="s">
+      <c r="G119" s="49"/>
+      <c r="H119" s="49"/>
+      <c r="I119" s="49"/>
+      <c r="J119" s="49"/>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>152</v>
+      </c>
+      <c r="B120" t="s">
         <v>220</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="C120" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D119">
-        <v>6</v>
-      </c>
-      <c r="E119">
+      <c r="D120">
+        <v>6</v>
+      </c>
+      <c r="E120" s="48">
         <v>53.64</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A120" s="3">
-        <v>152</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="C120" s="4" t="s">
-        <v>438</v>
-      </c>
-      <c r="D120" s="3">
-        <v>1</v>
-      </c>
-      <c r="E120" s="3"/>
-      <c r="F120" s="3"/>
-      <c r="G120" s="3"/>
-      <c r="H120" s="3"/>
-      <c r="I120" s="3"/>
-      <c r="J120" s="5">
-        <v>1010.36</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D121" s="3">
-        <v>2</v>
-      </c>
-      <c r="E121" s="3"/>
-      <c r="F121" s="3"/>
-      <c r="G121" s="3"/>
-      <c r="H121" s="3"/>
-      <c r="I121" s="3">
-        <v>-950.14</v>
-      </c>
-      <c r="J121" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="E121" s="49"/>
+      <c r="F121" s="49"/>
+      <c r="G121" s="49"/>
+      <c r="H121" s="49"/>
+      <c r="I121" s="49"/>
+      <c r="J121" s="49">
+        <v>1010.36</v>
+      </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D122" s="3">
-        <v>3</v>
-      </c>
-      <c r="E122" s="3"/>
-      <c r="F122" s="3"/>
-      <c r="G122" s="3"/>
-      <c r="H122" s="3">
+        <v>2</v>
+      </c>
+      <c r="E122" s="49"/>
+      <c r="F122" s="49"/>
+      <c r="G122" s="49"/>
+      <c r="H122" s="49"/>
+      <c r="I122" s="49">
         <v>-950.14</v>
       </c>
-      <c r="I122" s="3"/>
-      <c r="J122" s="3"/>
+      <c r="J122" s="49"/>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>416</v>
+        <v>442</v>
       </c>
       <c r="D123" s="3">
-        <v>4</v>
-      </c>
-      <c r="E123" s="3"/>
-      <c r="F123" s="3"/>
-      <c r="G123" s="3">
+        <v>3</v>
+      </c>
+      <c r="E123" s="49"/>
+      <c r="F123" s="49"/>
+      <c r="G123" s="49"/>
+      <c r="H123" s="49">
         <v>-950.14</v>
       </c>
-      <c r="H123" s="3"/>
-      <c r="I123" s="3"/>
-      <c r="J123" s="3"/>
+      <c r="I123" s="49"/>
+      <c r="J123" s="49"/>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B124" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="D124" s="3">
+        <v>4</v>
+      </c>
+      <c r="E124" s="49"/>
+      <c r="F124" s="49"/>
+      <c r="G124" s="49">
+        <v>-950.14</v>
+      </c>
+      <c r="H124" s="49"/>
+      <c r="I124" s="49"/>
+      <c r="J124" s="49"/>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A125" s="3">
+        <v>158</v>
+      </c>
+      <c r="B125" s="3" t="s">
         <v>444</v>
       </c>
-      <c r="C124" s="4" t="s">
+      <c r="C125" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="D124" s="3">
+      <c r="D125" s="3">
         <v>5</v>
       </c>
-      <c r="E124" s="3"/>
-      <c r="F124" s="3">
+      <c r="E125" s="49"/>
+      <c r="F125" s="49">
         <v>-950.14</v>
       </c>
-      <c r="G124" s="3"/>
-      <c r="H124" s="3"/>
-      <c r="I124" s="3"/>
-      <c r="J124" s="3"/>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A125">
-        <v>157</v>
-      </c>
-      <c r="B125" t="s">
+      <c r="G125" s="49"/>
+      <c r="H125" s="49"/>
+      <c r="I125" s="49"/>
+      <c r="J125" s="49"/>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>159</v>
+      </c>
+      <c r="B126" t="s">
         <v>445</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="C126" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="D125">
-        <v>6</v>
-      </c>
-      <c r="E125">
+      <c r="D126">
+        <v>6</v>
+      </c>
+      <c r="E126" s="48">
         <v>-950.14</v>
       </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A126" s="3">
-        <v>159</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="C126" s="4" t="s">
-        <v>447</v>
-      </c>
-      <c r="D126" s="3">
-        <v>2</v>
-      </c>
-      <c r="E126" s="3"/>
-      <c r="F126" s="3"/>
-      <c r="G126" s="3"/>
-      <c r="H126" s="3"/>
-      <c r="I126" s="5">
-        <v>1960.5</v>
-      </c>
-      <c r="J126" s="3"/>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D127" s="3">
-        <v>3</v>
-      </c>
-      <c r="E127" s="3"/>
-      <c r="F127" s="3"/>
-      <c r="G127" s="3"/>
-      <c r="H127" s="5">
+        <v>2</v>
+      </c>
+      <c r="E127" s="49"/>
+      <c r="F127" s="49"/>
+      <c r="G127" s="49"/>
+      <c r="H127" s="49"/>
+      <c r="I127" s="49">
         <v>1960.5</v>
       </c>
-      <c r="I127" s="3"/>
-      <c r="J127" s="3"/>
+      <c r="J127" s="49"/>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D128" s="3">
-        <v>4</v>
-      </c>
-      <c r="E128" s="3"/>
-      <c r="F128" s="3"/>
-      <c r="G128" s="5">
+        <v>3</v>
+      </c>
+      <c r="E128" s="49"/>
+      <c r="F128" s="49"/>
+      <c r="G128" s="49"/>
+      <c r="H128" s="49">
         <v>1960.5</v>
       </c>
-      <c r="H128" s="3"/>
-      <c r="I128" s="3"/>
-      <c r="J128" s="3"/>
+      <c r="I128" s="49"/>
+      <c r="J128" s="49"/>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B129" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="C129" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="D129" s="3">
+        <v>4</v>
+      </c>
+      <c r="E129" s="49"/>
+      <c r="F129" s="49"/>
+      <c r="G129" s="49">
+        <v>1960.5</v>
+      </c>
+      <c r="H129" s="49"/>
+      <c r="I129" s="49"/>
+      <c r="J129" s="49"/>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A130" s="3">
+        <v>164</v>
+      </c>
+      <c r="B130" s="3" t="s">
         <v>452</v>
       </c>
-      <c r="C129" s="4" t="s">
+      <c r="C130" s="4" t="s">
         <v>453</v>
       </c>
-      <c r="D129" s="3">
+      <c r="D130" s="3">
         <v>5</v>
       </c>
-      <c r="E129" s="3"/>
-      <c r="F129" s="5">
+      <c r="E130" s="49"/>
+      <c r="F130" s="49">
         <v>1960.5</v>
       </c>
-      <c r="G129" s="3"/>
-      <c r="H129" s="3"/>
-      <c r="I129" s="3"/>
-      <c r="J129" s="3"/>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A130">
-        <v>163</v>
-      </c>
-      <c r="B130" t="s">
+      <c r="G130" s="49"/>
+      <c r="H130" s="49"/>
+      <c r="I130" s="49"/>
+      <c r="J130" s="49"/>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>165</v>
+      </c>
+      <c r="B131" t="s">
         <v>454</v>
       </c>
-      <c r="C130" s="1" t="s">
+      <c r="C131" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="D130">
-        <v>6</v>
-      </c>
-      <c r="E130" s="2">
+      <c r="D131">
+        <v>6</v>
+      </c>
+      <c r="E131" s="48">
         <v>1960.5</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C131" s="1"/>
-      <c r="E131" s="2"/>
-    </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B132" s="7" t="s">
+      <c r="C132" s="1"/>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B133" s="7" t="s">
         <v>429</v>
       </c>
-      <c r="C132" s="7"/>
-      <c r="D132" s="7"/>
-      <c r="E132" s="7"/>
-      <c r="F132" s="7"/>
-      <c r="G132" s="7"/>
-      <c r="H132" s="7"/>
-      <c r="I132" s="7"/>
-      <c r="J132" s="8">
-        <f>SUM(J90:J131)</f>
-        <v>-153332.70000000001</v>
+      <c r="C133" s="7"/>
+      <c r="D133" s="7"/>
+      <c r="E133" s="50"/>
+      <c r="F133" s="50"/>
+      <c r="G133" s="50"/>
+      <c r="H133" s="50"/>
+      <c r="I133" s="50"/>
+      <c r="J133" s="50">
+        <f>SUM(J91:J132)</f>
+        <v>-53460.399999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>